<commit_message>
recommited with corrected files.
</commit_message>
<xml_diff>
--- a/机电系统设计成绩统计.xlsx
+++ b/机电系统设计成绩统计.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42">
   <si>
-    <t>机电系统设计课程设计评分记录表</t>
+    <t>机电系统设计课程设计评分记录表(Draft)</t>
   </si>
   <si>
     <t>编号</t>
@@ -1240,8 +1240,8 @@
   <sheetPr/>
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>

</xml_diff>